<commit_message>
convert settings to YAML
</commit_message>
<xml_diff>
--- a/data/20210323 Hinterkipper_de en_final_SAP.xlsx
+++ b/data/20210323 Hinterkipper_de en_final_SAP.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Merkmalswerte" sheetId="1" r:id="rId1"/>
+    <sheet name="Merkmale" sheetId="2" r:id="rId2"/>
+    <sheet name="Konditionen" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>ATINN</t>
   </si>
@@ -38,6 +40,21 @@
   </si>
   <si>
     <t>Wertebezeichnung (englisch)</t>
+  </si>
+  <si>
+    <t>Merkmalsbezeichnung (deutsch)</t>
+  </si>
+  <si>
+    <t>Merkmalsbezeichnung (englisch)</t>
+  </si>
+  <si>
+    <t>Kondition</t>
+  </si>
+  <si>
+    <t>deutsch</t>
+  </si>
+  <si>
+    <t>englisch</t>
   </si>
 </sst>
 </file>
@@ -433,4 +450,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>